<commit_message>
update scale factor in CIL debug
</commit_message>
<xml_diff>
--- a/flexlab/sw_mat_HIL2/HIL2_switch_matrix_13NF_bal_CILdebug.xlsx
+++ b/flexlab/sw_mat_HIL2/HIL2_switch_matrix_13NF_bal_CILdebug.xlsx
@@ -2196,34 +2196,34 @@
         <v>26</v>
       </c>
       <c r="C16" s="15">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D16" s="15">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E16" s="15">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F16" s="15">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G16" s="15">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H16" s="15">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="I16" s="15">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="J16" s="15">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="K16" s="15">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="L16" s="15">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>

</xml_diff>